<commit_message>
Miniscule changes; bringing github copy up to date with local
</commit_message>
<xml_diff>
--- a/Census Geog Reference.xlsx
+++ b/Census Geog Reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr date1904="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\Squeeze Project\FIPS SDWIS Matching\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\Squeeze Project\Census Geography Reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D912A8FD-CC71-4503-AB27-45E2BB79AC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49B2B0A-533B-440F-B48B-D7400049C307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2853" yWindow="2853" windowWidth="19200" windowHeight="10074" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3533" yWindow="3533" windowWidth="19200" windowHeight="10074" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Codebook" sheetId="8" r:id="rId1"/>
@@ -917,13 +917,13 @@
     <t>Wyandotte</t>
   </si>
   <si>
-    <t>Incorporated Places are independent of MCDs. There are a number of nongovernmental MCD types (i.e. gore, unorganized territory), with the Census of Governments generally considering the main municipal units to be cities, towns, and plantations.</t>
-  </si>
-  <si>
     <t>County governments have very limited powers in Maine; in places where municipal governments do not exist, the state provides services. Native American reservations are not counted as municipalities by the Census of Governments.</t>
   </si>
   <si>
     <t>T, PL, C</t>
+  </si>
+  <si>
+    <t>Incorporated Places are independent of MCDs. There are a number of nongovernmental MCD types (i.e. gore, unorganized territory) with the Census of Governments generally considering the main municipal units to be cities, towns, and plantations.</t>
   </si>
 </sst>
 </file>
@@ -1787,9 +1787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB36DFF3-2BC9-48D6-95D1-6CB50C7311A9}">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
@@ -1837,10 +1835,10 @@
   <dimension ref="A1:Q84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2320,7 +2318,7 @@
         <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D21" t="s">
         <v>120</v>
@@ -2335,10 +2333,10 @@
         <v>218</v>
       </c>
       <c r="J21" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K21" s="1" t="s">
         <v>285</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="28.7" x14ac:dyDescent="0.5">

</xml_diff>